<commit_message>
outsource unity project and add matlab scripts
</commit_message>
<xml_diff>
--- a/other/count_working_time.xlsx
+++ b/other/count_working_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Studium\Kogni_Tuebingen\Bachelorarbeit\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F4791C-429E-4435-9AE9-EDCB78D6A998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248E7B3E-CBF8-403A-B85C-AD387136C867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="-120" windowWidth="27750" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,7 +632,7 @@
   <dimension ref="B1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -666,7 +666,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="14">
         <f>SUM($E6:E40)</f>
-        <v>1.1493055555555554</v>
+        <v>2.3229166666666665</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -887,51 +887,123 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>44138</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>44139</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.875</v>
+      </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>44139</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>6.25E-2</v>
+      </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>44140</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.6875</v>
+      </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>44141</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.57638888888888895</v>
+      </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.7222222222222265E-2</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>44145</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.4513888888888889</v>
+      </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.472222222222221E-2</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>44145</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.9375</v>
+      </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>44146</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>